<commit_message>
feat: #19 Re-generated all the pages with current header and all tops by dictionaries.
</commit_message>
<xml_diff>
--- a/kgparserWeb/src/main/webapp/xlsx/voc-chars-top-by-races-count.xlsx
+++ b/kgparserWeb/src/main/webapp/xlsx/voc-chars-top-by-races-count.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4879" uniqueCount="4017">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4921" uniqueCount="4044">
   <si>
     <t>#</t>
   </si>
@@ -20,7 +20,7 @@
     <t>Логин</t>
   </si>
   <si>
-    <t>Профиль</t>
+    <t>Стат. по словарю</t>
   </si>
   <si>
     <t>Общий пробег</t>
@@ -12063,6 +12063,87 @@
   </si>
   <si>
     <t>1 ч. 6 мин. 53 сек.</t>
+  </si>
+  <si>
+    <t>1624–1637</t>
+  </si>
+  <si>
+    <t>jjjkeg</t>
+  </si>
+  <si>
+    <t>1 ч. 45 мин. 13 сек.</t>
+  </si>
+  <si>
+    <t>Chuchpek</t>
+  </si>
+  <si>
+    <t>1 ч. 8 мин. 29 сек.</t>
+  </si>
+  <si>
+    <t>i_vam98</t>
+  </si>
+  <si>
+    <t>1 ч. 28 мин. 16 сек.</t>
+  </si>
+  <si>
+    <t>-анахата-</t>
+  </si>
+  <si>
+    <t>1 ч. 56 мин. 34 сек.</t>
+  </si>
+  <si>
+    <t>Сергей-</t>
+  </si>
+  <si>
+    <t>1 ч. 42 мин. 43 сек.</t>
+  </si>
+  <si>
+    <t>iBumble</t>
+  </si>
+  <si>
+    <t>1 ч. 29 мин. 7 сек.</t>
+  </si>
+  <si>
+    <t>Модильяни</t>
+  </si>
+  <si>
+    <t>1 ч. 46 мин. 32 сек.</t>
+  </si>
+  <si>
+    <t>Da_f</t>
+  </si>
+  <si>
+    <t>Pill_Kates</t>
+  </si>
+  <si>
+    <t>1 ч. 18 мин. 24 сек.</t>
+  </si>
+  <si>
+    <t>Aleksandeer</t>
+  </si>
+  <si>
+    <t>1 ч. 28 мин. 4 сек.</t>
+  </si>
+  <si>
+    <t>gassar</t>
+  </si>
+  <si>
+    <t>2 ч. 24 мин. 48 сек.</t>
+  </si>
+  <si>
+    <t>дерик</t>
+  </si>
+  <si>
+    <t>1 ч. 33 мин. 9 сек.</t>
+  </si>
+  <si>
+    <t>_-Brain-_</t>
+  </si>
+  <si>
+    <t>1 ч. 26 мин. 5 сек.</t>
+  </si>
+  <si>
+    <t>sindek</t>
   </si>
 </sst>
 </file>
@@ -12647,7 +12728,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1624"/>
+  <dimension ref="A1:J1638"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -12655,7 +12736,7 @@
   <cols>
     <col min="1" max="1" width="15.625" customWidth="true"/>
     <col min="2" max="2" width="23.4375" customWidth="true"/>
-    <col min="3" max="3" width="11.71875" customWidth="true"/>
+    <col min="3" max="3" width="19.53125" customWidth="true"/>
     <col min="4" max="4" width="15.625" customWidth="true"/>
     <col min="5" max="5" width="15.625" customWidth="true"/>
     <col min="6" max="6" width="15.625" customWidth="true"/>
@@ -64631,6 +64712,454 @@
       </c>
       <c r="J1624" s="11" t="n">
         <v>40753.49685185185</v>
+      </c>
+    </row>
+    <row r="1625">
+      <c r="A1625" s="8" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1625" s="18" t="s">
+        <v>4018</v>
+      </c>
+      <c r="C1625" s="12" t="n">
+        <v>608451.0</v>
+      </c>
+      <c r="D1625" s="2" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E1625" s="2" t="n">
+        <v>198.0</v>
+      </c>
+      <c r="F1625" s="4" t="n">
+        <v>165.023</v>
+      </c>
+      <c r="G1625" s="4" t="n">
+        <v>2.48969</v>
+      </c>
+      <c r="H1625" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I1625" s="8" t="s">
+        <v>4019</v>
+      </c>
+      <c r="J1625" s="10" t="n">
+        <v>44180.65320601852</v>
+      </c>
+    </row>
+    <row r="1626">
+      <c r="A1626" s="9" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1626" s="23" t="s">
+        <v>4020</v>
+      </c>
+      <c r="C1626" s="13" t="n">
+        <v>540297.0</v>
+      </c>
+      <c r="D1626" s="3" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E1626" s="3" t="n">
+        <v>314.0</v>
+      </c>
+      <c r="F1626" s="5" t="n">
+        <v>258.79</v>
+      </c>
+      <c r="G1626" s="5" t="n">
+        <v>1.46826</v>
+      </c>
+      <c r="H1626" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I1626" s="9" t="s">
+        <v>4021</v>
+      </c>
+      <c r="J1626" s="11" t="n">
+        <v>43814.82949074074</v>
+      </c>
+    </row>
+    <row r="1627">
+      <c r="A1627" s="8" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1627" s="20" t="s">
+        <v>4022</v>
+      </c>
+      <c r="C1627" s="12" t="n">
+        <v>537000.0</v>
+      </c>
+      <c r="D1627" s="2" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E1627" s="2" t="n">
+        <v>264.0</v>
+      </c>
+      <c r="F1627" s="4" t="n">
+        <v>204.683</v>
+      </c>
+      <c r="G1627" s="4" t="n">
+        <v>1.58358</v>
+      </c>
+      <c r="H1627" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I1627" s="8" t="s">
+        <v>4023</v>
+      </c>
+      <c r="J1627" s="10" t="n">
+        <v>43851.81699074074</v>
+      </c>
+    </row>
+    <row r="1628">
+      <c r="A1628" s="9" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1628" s="21" t="s">
+        <v>4024</v>
+      </c>
+      <c r="C1628" s="13" t="n">
+        <v>507661.0</v>
+      </c>
+      <c r="D1628" s="3" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E1628" s="3" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="F1628" s="5" t="n">
+        <v>149.64</v>
+      </c>
+      <c r="G1628" s="5" t="n">
+        <v>3.64871</v>
+      </c>
+      <c r="H1628" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I1628" s="9" t="s">
+        <v>4025</v>
+      </c>
+      <c r="J1628" s="11" t="n">
+        <v>43077.72756944445</v>
+      </c>
+    </row>
+    <row r="1629">
+      <c r="A1629" s="8" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1629" s="14" t="s">
+        <v>4026</v>
+      </c>
+      <c r="C1629" s="12" t="n">
+        <v>492507.0</v>
+      </c>
+      <c r="D1629" s="2" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E1629" s="2" t="n">
+        <v>199.0</v>
+      </c>
+      <c r="F1629" s="4" t="n">
+        <v>170.56</v>
+      </c>
+      <c r="G1629" s="4" t="n">
+        <v>3.52205</v>
+      </c>
+      <c r="H1629" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I1629" s="8" t="s">
+        <v>4027</v>
+      </c>
+      <c r="J1629" s="10" t="n">
+        <v>43372.482094907406</v>
+      </c>
+    </row>
+    <row r="1630">
+      <c r="A1630" s="9" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1630" s="23" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C1630" s="13" t="n">
+        <v>452999.0</v>
+      </c>
+      <c r="D1630" s="3" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E1630" s="3" t="n">
+        <v>258.0</v>
+      </c>
+      <c r="F1630" s="5" t="n">
+        <v>194.591</v>
+      </c>
+      <c r="G1630" s="5" t="n">
+        <v>2.92169</v>
+      </c>
+      <c r="H1630" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I1630" s="9" t="s">
+        <v>4029</v>
+      </c>
+      <c r="J1630" s="11" t="n">
+        <v>43287.88721064815</v>
+      </c>
+    </row>
+    <row r="1631">
+      <c r="A1631" s="8" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1631" s="20" t="s">
+        <v>4030</v>
+      </c>
+      <c r="C1631" s="12" t="n">
+        <v>447649.0</v>
+      </c>
+      <c r="D1631" s="2" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E1631" s="2" t="n">
+        <v>198.0</v>
+      </c>
+      <c r="F1631" s="4" t="n">
+        <v>163.584</v>
+      </c>
+      <c r="G1631" s="4" t="n">
+        <v>2.43723</v>
+      </c>
+      <c r="H1631" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I1631" s="8" t="s">
+        <v>4031</v>
+      </c>
+      <c r="J1631" s="10" t="n">
+        <v>43134.921793981484</v>
+      </c>
+    </row>
+    <row r="1632">
+      <c r="A1632" s="9" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1632" s="23" t="s">
+        <v>4032</v>
+      </c>
+      <c r="C1632" s="13" t="n">
+        <v>423109.0</v>
+      </c>
+      <c r="D1632" s="3" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E1632" s="3" t="n">
+        <v>259.0</v>
+      </c>
+      <c r="F1632" s="5" t="n">
+        <v>208.127</v>
+      </c>
+      <c r="G1632" s="5" t="n">
+        <v>2.23887</v>
+      </c>
+      <c r="H1632" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I1632" s="9" t="s">
+        <v>3105</v>
+      </c>
+      <c r="J1632" s="11" t="n">
+        <v>44192.96068287037</v>
+      </c>
+    </row>
+    <row r="1633">
+      <c r="A1633" s="8" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1633" s="22" t="s">
+        <v>4033</v>
+      </c>
+      <c r="C1633" s="12" t="n">
+        <v>337026.0</v>
+      </c>
+      <c r="D1633" s="2" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E1633" s="2" t="n">
+        <v>255.0</v>
+      </c>
+      <c r="F1633" s="4" t="n">
+        <v>221.387</v>
+      </c>
+      <c r="G1633" s="4" t="n">
+        <v>4.20841</v>
+      </c>
+      <c r="H1633" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I1633" s="8" t="s">
+        <v>4034</v>
+      </c>
+      <c r="J1633" s="10" t="n">
+        <v>43612.583553240744</v>
+      </c>
+    </row>
+    <row r="1634">
+      <c r="A1634" s="9" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1634" s="23" t="s">
+        <v>4035</v>
+      </c>
+      <c r="C1634" s="13" t="n">
+        <v>310229.0</v>
+      </c>
+      <c r="D1634" s="3" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E1634" s="3" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="F1634" s="5" t="n">
+        <v>200.317</v>
+      </c>
+      <c r="G1634" s="5" t="n">
+        <v>3.77208</v>
+      </c>
+      <c r="H1634" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I1634" s="9" t="s">
+        <v>4036</v>
+      </c>
+      <c r="J1634" s="11" t="n">
+        <v>41325.530798611115</v>
+      </c>
+    </row>
+    <row r="1635">
+      <c r="A1635" s="8" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1635" s="18" t="s">
+        <v>4037</v>
+      </c>
+      <c r="C1635" s="12" t="n">
+        <v>300767.0</v>
+      </c>
+      <c r="D1635" s="2" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E1635" s="2" t="n">
+        <v>154.0</v>
+      </c>
+      <c r="F1635" s="4" t="n">
+        <v>122.434</v>
+      </c>
+      <c r="G1635" s="4" t="n">
+        <v>4.00829</v>
+      </c>
+      <c r="H1635" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I1635" s="8" t="s">
+        <v>4038</v>
+      </c>
+      <c r="J1635" s="10" t="n">
+        <v>42537.89738425926</v>
+      </c>
+    </row>
+    <row r="1636">
+      <c r="A1636" s="9" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1636" s="23" t="s">
+        <v>4039</v>
+      </c>
+      <c r="C1636" s="13" t="n">
+        <v>161743.0</v>
+      </c>
+      <c r="D1636" s="3" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E1636" s="3" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="F1636" s="5" t="n">
+        <v>192.324</v>
+      </c>
+      <c r="G1636" s="5" t="n">
+        <v>7.98453</v>
+      </c>
+      <c r="H1636" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I1636" s="9" t="s">
+        <v>4040</v>
+      </c>
+      <c r="J1636" s="11" t="n">
+        <v>41415.81079861111</v>
+      </c>
+    </row>
+    <row r="1637">
+      <c r="A1637" s="8" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1637" s="22" t="s">
+        <v>4041</v>
+      </c>
+      <c r="C1637" s="12" t="n">
+        <v>91773.0</v>
+      </c>
+      <c r="D1637" s="2" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E1637" s="2" t="n">
+        <v>264.0</v>
+      </c>
+      <c r="F1637" s="4" t="n">
+        <v>204.523</v>
+      </c>
+      <c r="G1637" s="4" t="n">
+        <v>6.36944</v>
+      </c>
+      <c r="H1637" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I1637" s="8" t="s">
+        <v>4042</v>
+      </c>
+      <c r="J1637" s="10" t="n">
+        <v>40078.55480324074</v>
+      </c>
+    </row>
+    <row r="1638">
+      <c r="A1638" s="9" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1638" s="23" t="s">
+        <v>4043</v>
+      </c>
+      <c r="C1638" s="13" t="n">
+        <v>91589.0</v>
+      </c>
+      <c r="D1638" s="3" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E1638" s="3" t="n">
+        <v>260.0</v>
+      </c>
+      <c r="F1638" s="5" t="n">
+        <v>192.884</v>
+      </c>
+      <c r="G1638" s="5" t="n">
+        <v>3.69296</v>
+      </c>
+      <c r="H1638" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I1638" s="9" t="s">
+        <v>3830</v>
+      </c>
+      <c r="J1638" s="11" t="n">
+        <v>39843.663773148146</v>
       </c>
     </row>
   </sheetData>
@@ -66258,6 +66787,20 @@
     <hyperlink ref="C1622" r:id="rId1621"/>
     <hyperlink ref="C1623" r:id="rId1622"/>
     <hyperlink ref="C1624" r:id="rId1623"/>
+    <hyperlink ref="C1625" r:id="rId1624"/>
+    <hyperlink ref="C1626" r:id="rId1625"/>
+    <hyperlink ref="C1627" r:id="rId1626"/>
+    <hyperlink ref="C1628" r:id="rId1627"/>
+    <hyperlink ref="C1629" r:id="rId1628"/>
+    <hyperlink ref="C1630" r:id="rId1629"/>
+    <hyperlink ref="C1631" r:id="rId1630"/>
+    <hyperlink ref="C1632" r:id="rId1631"/>
+    <hyperlink ref="C1633" r:id="rId1632"/>
+    <hyperlink ref="C1634" r:id="rId1633"/>
+    <hyperlink ref="C1635" r:id="rId1634"/>
+    <hyperlink ref="C1636" r:id="rId1635"/>
+    <hyperlink ref="C1637" r:id="rId1636"/>
+    <hyperlink ref="C1638" r:id="rId1637"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>